<commit_message>
fixed typo in excel db
</commit_message>
<xml_diff>
--- a/database_generator/DB_finale_v3.xlsx
+++ b/database_generator/DB_finale_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\covid_project\main\database_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E993F5D5-5773-4FC5-B2E4-892839D960E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDACB228-F144-496A-BFCD-49CA7909F9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1332" yWindow="2040" windowWidth="21444" windowHeight="10200" firstSheet="2" activeTab="3" xr2:uid="{EDF3959D-56DC-430F-A80D-5E497B9F704D}"/>
+    <workbookView xWindow="204" yWindow="1344" windowWidth="21444" windowHeight="10200" firstSheet="2" activeTab="3" xr2:uid="{EDF3959D-56DC-430F-A80D-5E497B9F704D}"/>
   </bookViews>
   <sheets>
     <sheet name="link utili" sheetId="4" r:id="rId1"/>
@@ -3846,9 +3846,6 @@
     <t>pop_density.tsv.avg</t>
   </si>
   <si>
-    <t>early_leavers_from_education_and_training_by_sex_percentage_nuts2.xlsx.avg</t>
-  </si>
-  <si>
     <t>farm_labour_force.tsv.sum</t>
   </si>
   <si>
@@ -3910,6 +3907,9 @@
   </si>
   <si>
     <t>causes_of_death_crude_death_rate_3year_average_by_nuts2.tsv.avg</t>
+  </si>
+  <si>
+    <t>early_leavers_from_education_and_training_by_sex_percentage_nuts2.tsv.avg</t>
   </si>
 </sst>
 </file>
@@ -6871,10 +6871,10 @@
   <dimension ref="A1:EF1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6882,21 +6882,21 @@
     <col min="1" max="1" width="21.6640625" style="66" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="66" customWidth="1"/>
     <col min="3" max="3" width="9.77734375" style="69" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="66" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="66" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="66" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="66" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" style="66" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="66" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.21875" style="66" customWidth="1"/>
-    <col min="9" max="9" width="42.88671875" style="66" customWidth="1"/>
-    <col min="10" max="10" width="35.77734375" style="66" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="66" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="66" customWidth="1"/>
-    <col min="13" max="13" width="12" style="62" customWidth="1"/>
-    <col min="14" max="14" width="14.21875" style="66" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" style="66" customWidth="1"/>
-    <col min="16" max="16" width="8.33203125" style="66" customWidth="1"/>
-    <col min="17" max="17" width="9.77734375" style="66" customWidth="1"/>
-    <col min="18" max="18" width="14.77734375" style="66" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" style="66" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="66" customWidth="1"/>
+    <col min="10" max="10" width="45.6640625" style="66" customWidth="1"/>
+    <col min="11" max="11" width="38.21875" style="66" customWidth="1"/>
+    <col min="12" max="12" width="41.5546875" style="66" customWidth="1"/>
+    <col min="13" max="13" width="46.5546875" style="62" customWidth="1"/>
+    <col min="14" max="14" width="43.21875" style="66" customWidth="1"/>
+    <col min="15" max="15" width="64.6640625" style="66" customWidth="1"/>
+    <col min="16" max="16" width="77.109375" style="66" customWidth="1"/>
+    <col min="17" max="17" width="79.6640625" style="66" customWidth="1"/>
+    <col min="18" max="18" width="55.77734375" style="66" customWidth="1"/>
     <col min="19" max="19" width="15.88671875" style="66" customWidth="1"/>
     <col min="20" max="20" width="11" style="66" customWidth="1"/>
     <col min="21" max="21" width="14.88671875" style="66" customWidth="1"/>
@@ -6907,9 +6907,9 @@
     <col min="26" max="26" width="10.44140625" style="66" customWidth="1"/>
     <col min="27" max="27" width="18.44140625" style="66" customWidth="1"/>
     <col min="28" max="28" width="30.88671875" style="66" customWidth="1"/>
-    <col min="29" max="29" width="30.6640625" style="66" customWidth="1"/>
-    <col min="30" max="30" width="14.109375" style="66" customWidth="1"/>
-    <col min="31" max="31" width="13.5546875" style="66" customWidth="1"/>
+    <col min="29" max="29" width="99.44140625" style="66" customWidth="1"/>
+    <col min="30" max="30" width="61.5546875" style="66" customWidth="1"/>
+    <col min="31" max="31" width="77.77734375" style="66" customWidth="1"/>
     <col min="32" max="16383" width="9.21875" style="66"/>
     <col min="16384" max="16384" width="9.21875" style="66" customWidth="1"/>
   </cols>
@@ -6940,73 +6940,73 @@
         <v>187</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>1232</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>1233</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>1234</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>1235</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>1236</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>1237</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>1238</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>1239</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>1240</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>1241</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>1242</v>
       </c>
       <c r="T1" s="78" t="s">
         <v>1230</v>
       </c>
       <c r="U1" s="6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>1243</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>1244</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>1245</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>1246</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>1247</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>1248</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>1249</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>1252</v>
+      </c>
+      <c r="AD1" s="6" t="s">
         <v>1250</v>
       </c>
-      <c r="AC1" s="6" t="s">
-        <v>1231</v>
-      </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>1251</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>1252</v>
       </c>
       <c r="AF1" s="6" t="s">
         <v>188</v>
@@ -13371,7 +13371,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
         <v>322</v>
       </c>
@@ -21025,7 +21025,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="137" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>600</v>
       </c>
@@ -21118,7 +21118,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="138" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>600</v>
       </c>
@@ -21211,7 +21211,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="139" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>600</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="142" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>600</v>
       </c>
@@ -21583,7 +21583,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="143" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>600</v>
       </c>
@@ -21676,7 +21676,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="144" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>600</v>
       </c>
@@ -24853,7 +24853,7 @@
       <c r="EE177" s="7"/>
       <c r="EF177" s="7"/>
     </row>
-    <row r="178" spans="1:136" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:136" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>741</v>
       </c>
@@ -26382,7 +26382,7 @@
       <c r="EE185" s="7"/>
       <c r="EF185" s="7"/>
     </row>
-    <row r="186" spans="1:136" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:136" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A186" s="23" t="s">
         <v>765</v>
       </c>
@@ -39441,7 +39441,7 @@
       <c r="EE252" s="7"/>
       <c r="EF252" s="7"/>
     </row>
-    <row r="253" spans="1:136" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:136" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A253" s="43" t="s">
         <v>66</v>
       </c>
@@ -41459,7 +41459,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="270" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A270" s="43" t="s">
         <v>66</v>
       </c>
@@ -42472,7 +42472,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="281" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A281" s="43" t="s">
         <v>66</v>
       </c>

</xml_diff>